<commit_message>
first draft of quest arrival
</commit_message>
<xml_diff>
--- a/pisar/data/personnel-details-demo.xlsx
+++ b/pisar/data/personnel-details-demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leonov\pisar\pisar\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pisar_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25879FF0-7A18-4C87-ADB2-D8D5312D924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6F947F-0820-4D07-8D92-26902BA54ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{C02CB7C7-9D3E-423C-A536-F2D74F3304F7}"/>
   </bookViews>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C1D9F2-D9D8-4BEB-B68E-9A3625C4731E}">
   <dimension ref="A1:CK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
-      <selection activeCell="CB1" sqref="CB1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>